<commit_message>
1. first version of SMPTE test pattern live wallpaper
</commit_message>
<xml_diff>
--- a/SMPTETestPatternFroyo/smpte.xlsx
+++ b/SMPTETestPatternFroyo/smpte.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
   <si>
     <t>Height</t>
   </si>
@@ -109,6 +109,45 @@
   </si>
   <si>
     <t xml:space="preserve"> drawRect Rect(133, 0 - 480, 60)</t>
+  </si>
+  <si>
+    <t>C0C0C0</t>
+  </si>
+  <si>
+    <t>C0C000</t>
+  </si>
+  <si>
+    <t>00C0C0</t>
+  </si>
+  <si>
+    <t>00C000</t>
+  </si>
+  <si>
+    <t>C000C0</t>
+  </si>
+  <si>
+    <t>C00000</t>
+  </si>
+  <si>
+    <t>0000C0</t>
+  </si>
+  <si>
+    <t>131313</t>
+  </si>
+  <si>
+    <t>00214C</t>
+  </si>
+  <si>
+    <t>FFFFFF</t>
+  </si>
+  <si>
+    <t>32006A</t>
+  </si>
+  <si>
+    <t>090909</t>
+  </si>
+  <si>
+    <t>1D1D1D</t>
   </si>
 </sst>
 </file>
@@ -147,12 +186,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,19 +487,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:H41"/>
+  <dimension ref="B1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7">
+    <row r="1" spans="2:9">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -476,7 +516,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:7">
+    <row r="2" spans="2:9">
       <c r="B2">
         <v>504</v>
       </c>
@@ -486,8 +526,11 @@
       <c r="G2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:7">
+      <c r="I2" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9">
       <c r="B3">
         <v>294</v>
       </c>
@@ -505,8 +548,11 @@
       <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="2:7">
+      <c r="I3" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
       <c r="B4">
         <v>294</v>
       </c>
@@ -514,18 +560,21 @@
         <v>96</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:D13" si="0">B4/$B$2</f>
+        <f t="shared" ref="D4:D26" si="0">B4/$B$2</f>
         <v>0.58333333333333337</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" ref="E4:E13" si="1">C4/$C$2</f>
+        <f t="shared" ref="E4:E26" si="1">C4/$C$2</f>
         <v>0.10714285714285714</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="2:7">
+      <c r="I4" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
       <c r="B5">
         <v>42</v>
       </c>
@@ -543,8 +592,11 @@
       <c r="G5" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="2:7">
+      <c r="I5" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
       <c r="C6">
         <v>576</v>
       </c>
@@ -559,8 +611,11 @@
       <c r="G6" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="2:7">
+      <c r="I6" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
       <c r="B7">
         <v>126</v>
       </c>
@@ -578,13 +633,16 @@
       <c r="G7" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="2:7">
+      <c r="I7" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
       <c r="B8">
         <v>126</v>
       </c>
       <c r="C8">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="D8" s="1">
         <f>B8/$B$2</f>
@@ -592,18 +650,21 @@
       </c>
       <c r="E8" s="1">
         <f t="shared" si="1"/>
-        <v>0.1875</v>
+        <v>0.16071428571428573</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="2:7">
+      <c r="I8" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
       <c r="B9">
         <v>126</v>
       </c>
       <c r="C9">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
@@ -611,13 +672,16 @@
       </c>
       <c r="E9" s="1">
         <f t="shared" si="1"/>
-        <v>0.21875</v>
+        <v>0.21428571428571427</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="2:7">
+      <c r="I9" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
       <c r="C10">
         <v>90</v>
       </c>
@@ -632,8 +696,11 @@
       <c r="G10" s="2">
         <v>696969</v>
       </c>
-    </row>
-    <row r="11" spans="2:7">
+      <c r="I10" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
       <c r="C11">
         <v>30</v>
       </c>
@@ -648,8 +715,11 @@
       <c r="G11" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="2:7">
+      <c r="I11" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
       <c r="C12">
         <v>96</v>
       </c>
@@ -664,8 +734,11 @@
       <c r="G12" s="2">
         <v>52550</v>
       </c>
-    </row>
-    <row r="13" spans="2:7">
+      <c r="I12" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
       <c r="C13">
         <v>112</v>
       </c>
@@ -680,93 +753,265 @@
       <c r="G13" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="2:7">
+      <c r="I13" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14">
+        <v>504</v>
+      </c>
+      <c r="C14">
+        <v>672</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="G14" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="2:7">
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="I14" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15">
+        <v>336</v>
+      </c>
+      <c r="C15">
+        <v>96</v>
+      </c>
+      <c r="D15" s="1">
+        <f>B15/$B$14</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E15" s="1">
+        <f>C15/$C$14</f>
+        <v>0.14285714285714285</v>
+      </c>
       <c r="G15" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="2:7">
+      <c r="I15" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16">
+        <v>42</v>
+      </c>
+      <c r="C16">
+        <v>96</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" si="1"/>
+        <v>0.10714285714285714</v>
+      </c>
       <c r="G16" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="7:8">
+      <c r="I16" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17">
+        <v>126</v>
+      </c>
+      <c r="C17">
+        <v>120</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="1"/>
+        <v>0.13392857142857142</v>
+      </c>
       <c r="G17" s="2">
         <v>50505</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="7:8">
+      <c r="I17" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18">
+        <v>126</v>
+      </c>
+      <c r="C18">
+        <v>32</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="1"/>
+        <v>3.5714285714285712E-2</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19">
+        <v>126</v>
+      </c>
+      <c r="C19">
+        <v>96</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="1"/>
+        <v>0.10714285714285714</v>
+      </c>
       <c r="G19" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="7:8">
+      <c r="I19" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="G20" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="7:8">
+      <c r="I20" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="G21" s="2">
         <v>50505</v>
       </c>
-    </row>
-    <row r="22" spans="7:8">
+      <c r="I21" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="G22" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="7:8">
+      <c r="I22" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="G23" s="2">
         <v>50505</v>
       </c>
-    </row>
-    <row r="24" spans="7:8">
+      <c r="I23" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="G24" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="7:8">
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="D25" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="G25" s="2">
         <v>50505</v>
       </c>
-    </row>
-    <row r="26" spans="7:8">
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="D26" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="G26" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="27" spans="7:8">
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="2:9">
       <c r="G27" s="2">
         <v>50505</v>
       </c>
-    </row>
-    <row r="28" spans="7:8">
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="2:9">
       <c r="G28" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="29" spans="7:8">
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="2:9">
       <c r="G29" s="2">
         <v>50505</v>
       </c>
-    </row>
-    <row r="30" spans="7:8">
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="2:9">
       <c r="G30" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="I30" s="3"/>
     </row>
     <row r="33" spans="2:7">
       <c r="B33" t="s">
@@ -794,10 +1039,6 @@
     <row r="36" spans="2:7">
       <c r="B36" t="s">
         <v>26</v>
-      </c>
-      <c r="G36">
-        <f>480/8</f>
-        <v>60</v>
       </c>
     </row>
     <row r="38" spans="2:7">

</xml_diff>

<commit_message>
1. added support for three test patterns: SMPTE 16x9, SMPTE 4x3, EBU 2. moved colors to XML resource file
</commit_message>
<xml_diff>
--- a/SMPTETestPatternFroyo/smpte.xlsx
+++ b/SMPTETestPatternFroyo/smpte.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
   <si>
     <t>Height</t>
   </si>
@@ -148,6 +148,24 @@
   </si>
   <si>
     <t>1D1D1D</t>
+  </si>
+  <si>
+    <t>BFBFBF</t>
+  </si>
+  <si>
+    <t>BFBF00</t>
+  </si>
+  <si>
+    <t>00BFBF</t>
+  </si>
+  <si>
+    <t>00BF00</t>
+  </si>
+  <si>
+    <t>BF0000</t>
+  </si>
+  <si>
+    <t>0000BF</t>
   </si>
 </sst>
 </file>
@@ -490,7 +508,7 @@
   <dimension ref="B1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -803,12 +821,12 @@
         <v>96</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D16:D19" si="2">B16/$B$14</f>
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" si="1"/>
-        <v>0.10714285714285714</v>
+        <f t="shared" ref="E16:E19" si="3">C16/$C$14</f>
+        <v>0.14285714285714285</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>16</v>
@@ -825,12 +843,12 @@
         <v>120</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" si="1"/>
-        <v>0.13392857142857142</v>
+        <f t="shared" si="3"/>
+        <v>0.17857142857142858</v>
       </c>
       <c r="G17" s="2">
         <v>50505</v>
@@ -850,12 +868,12 @@
         <v>32</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" si="1"/>
-        <v>3.5714285714285712E-2</v>
+        <f t="shared" si="3"/>
+        <v>4.7619047619047616E-2</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>41</v>
@@ -869,12 +887,12 @@
         <v>96</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" si="1"/>
-        <v>0.10714285714285714</v>
+        <f t="shared" si="3"/>
+        <v>0.14285714285714285</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>18</v>
@@ -884,14 +902,8 @@
       </c>
     </row>
     <row r="20" spans="2:9">
-      <c r="D20" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E20" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
       <c r="G20" s="2" t="s">
         <v>19</v>
       </c>
@@ -900,14 +912,14 @@
       </c>
     </row>
     <row r="21" spans="2:9">
-      <c r="D21" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E21" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+      <c r="B21">
+        <v>150</v>
+      </c>
+      <c r="C21">
+        <v>200</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
       <c r="G21" s="2">
         <v>50505</v>
       </c>
@@ -916,13 +928,19 @@
       </c>
     </row>
     <row r="22" spans="2:9">
+      <c r="B22">
+        <v>150</v>
+      </c>
+      <c r="C22">
+        <v>25</v>
+      </c>
       <c r="D22" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>B22/$B$21</f>
+        <v>1</v>
       </c>
       <c r="E22" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>C22/$C$21</f>
+        <v>0.125</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>20</v>
@@ -933,11 +951,11 @@
     </row>
     <row r="23" spans="2:9">
       <c r="D23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D23:D26" si="4">B23/$B$21</f>
         <v>0</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="E23:E26" si="5">C23/$C$21</f>
         <v>0</v>
       </c>
       <c r="G23" s="2">
@@ -949,11 +967,11 @@
     </row>
     <row r="24" spans="2:9">
       <c r="D24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G24" s="2">
@@ -963,55 +981,72 @@
     </row>
     <row r="25" spans="2:9">
       <c r="D25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G25" s="2">
         <v>50505</v>
       </c>
-      <c r="I25" s="3"/>
+      <c r="I25" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="26" spans="2:9">
       <c r="D26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I26" s="3"/>
+      <c r="I26" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="27" spans="2:9">
       <c r="G27" s="2">
         <v>50505</v>
       </c>
-      <c r="I27" s="3"/>
+      <c r="I27" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="28" spans="2:9">
       <c r="G28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I28" s="3"/>
+      <c r="I28" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="29" spans="2:9">
       <c r="G29" s="2">
         <v>50505</v>
       </c>
-      <c r="I29" s="3"/>
+      <c r="I29" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="30" spans="2:9">
       <c r="G30" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I30" s="3"/>
+      <c r="I30" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="I31">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="2:7">
       <c r="B33" t="s">

</xml_diff>